<commit_message>
Corrected errors in the combined model
</commit_message>
<xml_diff>
--- a/Data/kidney/Parameters_kidney.xlsx
+++ b/Data/kidney/Parameters_kidney.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cm1om\Documents\1. Research\1.  Cancer\1.  Bladder\Bladder_cancer_model\Data\kidney\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cm1om\Documents\1. Research\1.Cancer\1.Bladder\Bladder_cancer_model\Data\kidney\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E733BE-BE7F-4434-9FAC-A63CA979F3EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C7CD0D-A0DF-4A9D-997E-C873C149A0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{1AD6D928-CCB7-482A-A47C-26785A7D3A52}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1AD6D928-CCB7-482A-A47C-26785A7D3A52}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -2137,7 +2137,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="214">
+  <cellXfs count="215">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2463,6 +2463,7 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -4527,8 +4528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8694223C-410D-4023-9128-3FD5F8A481E4}">
   <dimension ref="A1:Z56"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4573,17 +4574,17 @@
       <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="191" t="s">
+      <c r="H1" s="192" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="191"/>
+      <c r="I1" s="192"/>
       <c r="J1" s="60" t="s">
         <v>221</v>
       </c>
-      <c r="K1" s="192" t="s">
+      <c r="K1" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="192"/>
+      <c r="L1" s="193"/>
       <c r="M1" s="2" t="s">
         <v>7</v>
       </c>
@@ -6162,7 +6163,7 @@
         <v>0.99642799999999998</v>
       </c>
       <c r="I34" s="117">
-        <f t="shared" ref="I34:I38" si="9">(L34-K34)/(2*NORMINV(0.975,0,1))</f>
+        <f t="shared" ref="I34" si="9">(L34-K34)/(2*NORMINV(0.975,0,1))</f>
         <v>7.4593207402382552E-4</v>
       </c>
       <c r="J34" s="117">
@@ -6249,32 +6250,35 @@
       <c r="D36" s="117" t="s">
         <v>189</v>
       </c>
-      <c r="E36" s="117">
-        <v>-0.08</v>
-      </c>
-      <c r="F36" s="117" t="s">
+      <c r="E36" s="191">
+        <f>0.763/0.84606</f>
+        <v>0.90182729357255986</v>
+      </c>
+      <c r="F36" s="191" t="s">
         <v>178</v>
       </c>
-      <c r="G36" s="117">
+      <c r="G36" s="191">
         <v>5</v>
       </c>
-      <c r="H36" s="117">
-        <f t="shared" ref="H36:H38" si="10">E36</f>
-        <v>-0.08</v>
-      </c>
-      <c r="I36" s="117">
-        <f t="shared" si="9"/>
-        <v>4.3368143838595594E-2</v>
-      </c>
-      <c r="J36" s="117">
+      <c r="H36" s="191">
         <f>E36</f>
-        <v>-0.08</v>
-      </c>
-      <c r="K36" s="117">
-        <v>-0.3</v>
-      </c>
-      <c r="L36" s="117">
-        <v>-0.13</v>
+        <v>0.90182729357255986</v>
+      </c>
+      <c r="I36" s="191">
+        <f>(L36-K36)/(2*NORMINV(0.975,0,1))</f>
+        <v>2.3744845703419688E-2</v>
+      </c>
+      <c r="J36" s="191">
+        <f t="shared" si="8"/>
+        <v>0.90182729357255986</v>
+      </c>
+      <c r="K36" s="191">
+        <f>0.71178/0.83292</f>
+        <v>0.85455986169139886</v>
+      </c>
+      <c r="L36" s="191">
+        <f>0.81422/0.85921</f>
+        <v>0.9476379464857253</v>
       </c>
       <c r="M36" s="117"/>
       <c r="N36" s="117" t="s">
@@ -6296,32 +6300,35 @@
       <c r="D37" s="117" t="s">
         <v>191</v>
       </c>
-      <c r="E37" s="117">
-        <v>-0.18</v>
-      </c>
-      <c r="F37" s="117" t="s">
+      <c r="E37" s="191">
+        <f>0.74698/0.84606</f>
+        <v>0.88289246625534823</v>
+      </c>
+      <c r="F37" s="191" t="s">
         <v>178</v>
       </c>
-      <c r="G37" s="117">
+      <c r="G37" s="191">
         <v>5</v>
       </c>
-      <c r="H37" s="117">
-        <f t="shared" si="10"/>
-        <v>-0.18</v>
-      </c>
-      <c r="I37" s="117">
-        <f t="shared" si="9"/>
-        <v>6.1225614830958487E-2</v>
-      </c>
-      <c r="J37" s="117">
+      <c r="H37" s="191">
+        <f>E37</f>
+        <v>0.88289246625534823</v>
+      </c>
+      <c r="I37" s="191">
+        <f>(L37-K37)/(2*NORMINV(0.975,0,1))</f>
+        <v>3.5594818478965271E-2</v>
+      </c>
+      <c r="J37" s="191">
         <f t="shared" si="8"/>
-        <v>-0.18</v>
-      </c>
-      <c r="K37" s="117">
-        <v>-0.3</v>
-      </c>
-      <c r="L37" s="117">
-        <v>-0.06</v>
+        <v>0.88289246625534823</v>
+      </c>
+      <c r="K37" s="191">
+        <f>0.67309/0.83292</f>
+        <v>0.80810882197569989</v>
+      </c>
+      <c r="L37" s="191">
+        <f>0.81422/0.85921</f>
+        <v>0.9476379464857253</v>
       </c>
       <c r="M37" s="117"/>
       <c r="N37" s="117" t="s">
@@ -6343,32 +6350,30 @@
       <c r="D38" s="117" t="s">
         <v>194</v>
       </c>
-      <c r="E38" s="117">
-        <v>0</v>
-      </c>
-      <c r="F38" s="117" t="s">
+      <c r="E38" s="191">
+        <v>1</v>
+      </c>
+      <c r="F38" s="191" t="s">
         <v>171</v>
       </c>
-      <c r="G38" s="117">
+      <c r="G38" s="191">
         <v>6</v>
       </c>
-      <c r="H38" s="117">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I38" s="117">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="J38" s="117">
+      <c r="H38" s="191">
+        <v>1</v>
+      </c>
+      <c r="I38" s="191">
+        <v>1</v>
+      </c>
+      <c r="J38" s="191">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="K38" s="117">
-        <v>0</v>
-      </c>
-      <c r="L38" s="117">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K38" s="191">
+        <v>1</v>
+      </c>
+      <c r="L38" s="191">
+        <v>1</v>
       </c>
       <c r="M38" s="117"/>
       <c r="N38" s="117" t="s">
@@ -6415,7 +6420,7 @@
         <v>1911.0774265016828</v>
       </c>
       <c r="L39" s="117">
-        <f t="shared" ref="L39" si="11">_xlfn.GAMMA.INV(0.975,H39,I39)</f>
+        <f t="shared" ref="L39" si="10">_xlfn.GAMMA.INV(0.975,H39,I39)</f>
         <v>2830.9839248261155</v>
       </c>
       <c r="M39" s="50"/>
@@ -6460,7 +6465,7 @@
         <v>-57.2</v>
       </c>
       <c r="K40" s="117">
-        <f t="shared" ref="K40:K48" si="12">E40-(I40*NORMINV(0.975,0,1))</f>
+        <f t="shared" ref="K40:K48" si="11">E40-(I40*NORMINV(0.975,0,1))</f>
         <v>-68.410993991569114</v>
       </c>
       <c r="L40" s="117">
@@ -6497,7 +6502,7 @@
         <v>5</v>
       </c>
       <c r="H41" s="117">
-        <f t="shared" ref="H41:H42" si="13">E41</f>
+        <f t="shared" ref="H41:H42" si="12">E41</f>
         <v>-242</v>
       </c>
       <c r="I41" s="117">
@@ -6509,7 +6514,7 @@
         <v>-242</v>
       </c>
       <c r="K41" s="117">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-289.4311284258693</v>
       </c>
       <c r="L41" s="117">
@@ -6546,7 +6551,7 @@
         <v>5</v>
       </c>
       <c r="H42" s="117">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>-921.4</v>
       </c>
       <c r="I42" s="117">
@@ -6558,7 +6563,7 @@
         <v>-921.4</v>
       </c>
       <c r="K42" s="117">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-1101.9910815355206</v>
       </c>
       <c r="L42" s="117">
@@ -6607,7 +6612,7 @@
         <v>-1514</v>
       </c>
       <c r="K43" s="117">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-1810.7385472593642</v>
       </c>
       <c r="L43" s="117">
@@ -6656,7 +6661,7 @@
         <v>1446.8</v>
       </c>
       <c r="K44" s="59">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>1163.2324107167451</v>
       </c>
       <c r="L44" s="59">
@@ -6693,7 +6698,7 @@
         <v>5</v>
       </c>
       <c r="H45" s="117">
-        <f t="shared" ref="H45:H48" si="14">E45</f>
+        <f t="shared" ref="H45:H48" si="13">E45</f>
         <v>1676.1</v>
       </c>
       <c r="I45" s="58">
@@ -6705,11 +6710,11 @@
         <v>1676.1</v>
       </c>
       <c r="K45" s="59">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>1347.5904365512415</v>
       </c>
       <c r="L45" s="59">
-        <f t="shared" ref="L45:L48" si="15">E45+(I45*NORMINV(0.975,0,1))</f>
+        <f t="shared" ref="L45:L48" si="14">E45+(I45*NORMINV(0.975,0,1))</f>
         <v>2004.6095634487583</v>
       </c>
       <c r="M45" s="117"/>
@@ -6742,11 +6747,11 @@
         <v>5</v>
       </c>
       <c r="H46" s="117">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>3956.7</v>
       </c>
       <c r="I46" s="58">
-        <f t="shared" ref="I46:I48" si="16">H46*0.1</f>
+        <f t="shared" ref="I46:I48" si="15">H46*0.1</f>
         <v>395.67</v>
       </c>
       <c r="J46" s="117">
@@ -6754,11 +6759,11 @@
         <v>3956.7</v>
       </c>
       <c r="K46" s="59">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>3181.2010502370367</v>
       </c>
       <c r="L46" s="59">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>4732.1989497629629</v>
       </c>
       <c r="M46" s="117"/>
@@ -6791,11 +6796,11 @@
         <v>5</v>
       </c>
       <c r="H47" s="117">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>5406.9</v>
       </c>
       <c r="I47" s="58">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>540.68999999999994</v>
       </c>
       <c r="J47" s="117">
@@ -6803,11 +6808,11 @@
         <v>5406.9</v>
       </c>
       <c r="K47" s="59">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>4347.167073199038</v>
       </c>
       <c r="L47" s="59">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>6466.6329268009613</v>
       </c>
       <c r="M47" s="117"/>
@@ -6840,11 +6845,11 @@
         <v>5</v>
       </c>
       <c r="H48" s="117">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>1217.4000000000001</v>
       </c>
       <c r="I48" s="58">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>121.74000000000001</v>
       </c>
       <c r="J48" s="117">
@@ -6852,11 +6857,11 @@
         <v>1217.4000000000001</v>
       </c>
       <c r="K48" s="59">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>978.79398452209398</v>
       </c>
       <c r="L48" s="59">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1456.0060154779062</v>
       </c>
       <c r="M48" s="117"/>
@@ -9597,31 +9602,31 @@
       </c>
     </row>
     <row r="2" spans="1:20" s="44" customFormat="1" ht="12.75">
-      <c r="A2" s="209" t="s">
+      <c r="A2" s="210" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="211" t="s">
+      <c r="B2" s="212" t="s">
         <v>131</v>
       </c>
-      <c r="C2" s="212" t="s">
+      <c r="C2" s="213" t="s">
         <v>230</v>
       </c>
-      <c r="D2" s="212"/>
-      <c r="E2" s="212"/>
-      <c r="F2" s="212"/>
-      <c r="G2" s="212"/>
+      <c r="D2" s="213"/>
+      <c r="E2" s="213"/>
+      <c r="F2" s="213"/>
+      <c r="G2" s="213"/>
       <c r="H2" s="72"/>
-      <c r="I2" s="212" t="s">
+      <c r="I2" s="213" t="s">
         <v>231</v>
       </c>
-      <c r="J2" s="212"/>
-      <c r="K2" s="212"/>
-      <c r="L2" s="212"/>
-      <c r="M2" s="212"/>
+      <c r="J2" s="213"/>
+      <c r="K2" s="213"/>
+      <c r="L2" s="213"/>
+      <c r="M2" s="213"/>
     </row>
     <row r="3" spans="1:20" s="44" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A3" s="210"/>
-      <c r="B3" s="210"/>
+      <c r="A3" s="211"/>
+      <c r="B3" s="211"/>
       <c r="C3" s="73" t="s">
         <v>232</v>
       </c>
@@ -9698,12 +9703,12 @@
       <c r="M4" s="79">
         <v>11.9</v>
       </c>
-      <c r="O4" s="205" t="s">
+      <c r="O4" s="206" t="s">
         <v>235</v>
       </c>
-      <c r="P4" s="205"/>
-      <c r="Q4" s="205"/>
-      <c r="R4" s="205"/>
+      <c r="P4" s="206"/>
+      <c r="Q4" s="206"/>
+      <c r="R4" s="206"/>
     </row>
     <row r="5" spans="1:20" s="44" customFormat="1" ht="12.75">
       <c r="A5" s="78" t="s">
@@ -9795,52 +9800,52 @@
       </c>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="193" t="s">
+      <c r="A10" s="194" t="s">
         <v>238</v>
       </c>
-      <c r="B10" s="194"/>
-      <c r="C10" s="194"/>
-      <c r="D10" s="194"/>
-      <c r="E10" s="194"/>
-      <c r="F10" s="194"/>
-      <c r="G10" s="194"/>
-      <c r="H10" s="194"/>
-      <c r="I10" s="194"/>
-      <c r="J10" s="194"/>
-      <c r="K10" s="194"/>
-      <c r="L10" s="194"/>
-      <c r="M10" s="194"/>
-      <c r="N10" s="194"/>
-      <c r="O10" s="194"/>
-      <c r="P10" s="194"/>
-      <c r="Q10" s="194"/>
-      <c r="R10" s="194"/>
-      <c r="S10" s="194"/>
-      <c r="T10" s="194"/>
+      <c r="B10" s="195"/>
+      <c r="C10" s="195"/>
+      <c r="D10" s="195"/>
+      <c r="E10" s="195"/>
+      <c r="F10" s="195"/>
+      <c r="G10" s="195"/>
+      <c r="H10" s="195"/>
+      <c r="I10" s="195"/>
+      <c r="J10" s="195"/>
+      <c r="K10" s="195"/>
+      <c r="L10" s="195"/>
+      <c r="M10" s="195"/>
+      <c r="N10" s="195"/>
+      <c r="O10" s="195"/>
+      <c r="P10" s="195"/>
+      <c r="Q10" s="195"/>
+      <c r="R10" s="195"/>
+      <c r="S10" s="195"/>
+      <c r="T10" s="195"/>
     </row>
     <row r="12" spans="1:20">
-      <c r="A12" s="206" t="s">
+      <c r="A12" s="207" t="s">
         <v>239</v>
       </c>
-      <c r="B12" s="194"/>
-      <c r="C12" s="194"/>
-      <c r="D12" s="194"/>
-      <c r="E12" s="194"/>
-      <c r="F12" s="194"/>
-      <c r="G12" s="194"/>
-      <c r="H12" s="194"/>
-      <c r="I12" s="194"/>
-      <c r="J12" s="194"/>
-      <c r="K12" s="194"/>
-      <c r="L12" s="194"/>
-      <c r="M12" s="194"/>
-      <c r="N12" s="194"/>
-      <c r="O12" s="194"/>
-      <c r="P12" s="194"/>
-      <c r="Q12" s="194"/>
-      <c r="R12" s="194"/>
-      <c r="S12" s="194"/>
-      <c r="T12" s="194"/>
+      <c r="B12" s="195"/>
+      <c r="C12" s="195"/>
+      <c r="D12" s="195"/>
+      <c r="E12" s="195"/>
+      <c r="F12" s="195"/>
+      <c r="G12" s="195"/>
+      <c r="H12" s="195"/>
+      <c r="I12" s="195"/>
+      <c r="J12" s="195"/>
+      <c r="K12" s="195"/>
+      <c r="L12" s="195"/>
+      <c r="M12" s="195"/>
+      <c r="N12" s="195"/>
+      <c r="O12" s="195"/>
+      <c r="P12" s="195"/>
+      <c r="Q12" s="195"/>
+      <c r="R12" s="195"/>
+      <c r="S12" s="195"/>
+      <c r="T12" s="195"/>
     </row>
     <row r="14" spans="1:20" ht="51">
       <c r="A14" s="84" t="s">
@@ -10265,17 +10270,17 @@
       </c>
     </row>
     <row r="28" spans="1:18">
-      <c r="A28" s="207" t="s">
+      <c r="A28" s="208" t="s">
         <v>251</v>
       </c>
-      <c r="B28" s="207"/>
-      <c r="C28" s="207"/>
-      <c r="D28" s="207"/>
-      <c r="E28" s="207"/>
-      <c r="F28" s="207"/>
-      <c r="G28" s="207"/>
-      <c r="H28" s="207"/>
-      <c r="I28" s="207"/>
+      <c r="B28" s="208"/>
+      <c r="C28" s="208"/>
+      <c r="D28" s="208"/>
+      <c r="E28" s="208"/>
+      <c r="F28" s="208"/>
+      <c r="G28" s="208"/>
+      <c r="H28" s="208"/>
+      <c r="I28" s="208"/>
       <c r="O28" s="88" t="s">
         <v>144</v>
       </c>
@@ -10293,17 +10298,17 @@
       </c>
     </row>
     <row r="29" spans="1:18">
-      <c r="A29" s="208" t="s">
+      <c r="A29" s="209" t="s">
         <v>252</v>
       </c>
-      <c r="B29" s="208"/>
-      <c r="C29" s="208"/>
-      <c r="D29" s="208"/>
-      <c r="E29" s="208"/>
-      <c r="F29" s="208"/>
-      <c r="G29" s="208"/>
-      <c r="H29" s="208"/>
-      <c r="I29" s="208"/>
+      <c r="B29" s="209"/>
+      <c r="C29" s="209"/>
+      <c r="D29" s="209"/>
+      <c r="E29" s="209"/>
+      <c r="F29" s="209"/>
+      <c r="G29" s="209"/>
+      <c r="H29" s="209"/>
+      <c r="I29" s="209"/>
       <c r="N29" s="44" t="s">
         <v>152</v>
       </c>
@@ -10340,17 +10345,17 @@
       </c>
     </row>
     <row r="31" spans="1:18">
-      <c r="A31" s="213" t="s">
+      <c r="A31" s="214" t="s">
         <v>254</v>
       </c>
-      <c r="B31" s="213"/>
-      <c r="C31" s="213"/>
-      <c r="D31" s="213"/>
-      <c r="E31" s="213"/>
-      <c r="F31" s="213"/>
-      <c r="G31" s="213"/>
-      <c r="H31" s="213"/>
-      <c r="I31" s="213"/>
+      <c r="B31" s="214"/>
+      <c r="C31" s="214"/>
+      <c r="D31" s="214"/>
+      <c r="E31" s="214"/>
+      <c r="F31" s="214"/>
+      <c r="G31" s="214"/>
+      <c r="H31" s="214"/>
+      <c r="I31" s="214"/>
       <c r="N31" s="44"/>
       <c r="O31" s="88" t="s">
         <v>141</v>
@@ -10369,14 +10374,14 @@
       </c>
     </row>
     <row r="32" spans="1:18">
-      <c r="E32" s="204" t="s">
+      <c r="E32" s="205" t="s">
         <v>139</v>
       </c>
-      <c r="F32" s="204"/>
-      <c r="G32" s="204" t="s">
+      <c r="F32" s="205"/>
+      <c r="G32" s="205" t="s">
         <v>158</v>
       </c>
-      <c r="H32" s="204"/>
+      <c r="H32" s="205"/>
       <c r="N32" s="44"/>
       <c r="O32" s="88" t="s">
         <v>142</v>
@@ -11971,8 +11976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F32D2E0-32A8-4C75-8C98-9C12E5C1268D}">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:F51"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12301,8 +12306,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="67">
-        <f>parameters!G13</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" s="69">
         <f>parameters!H13</f>
@@ -12896,7 +12900,7 @@
       </c>
       <c r="B36" s="68">
         <f>parameters!E36</f>
-        <v>-0.08</v>
+        <v>0.90182729357255986</v>
       </c>
       <c r="C36" s="67">
         <f>parameters!G36</f>
@@ -12904,15 +12908,15 @@
       </c>
       <c r="D36" s="69">
         <f>parameters!H36</f>
-        <v>-0.08</v>
+        <v>0.90182729357255986</v>
       </c>
       <c r="E36" s="69">
         <f>parameters!I36</f>
-        <v>4.3368143838595594E-2</v>
+        <v>2.3744845703419688E-2</v>
       </c>
       <c r="F36" s="69">
         <f>parameters!J36</f>
-        <v>-0.08</v>
+        <v>0.90182729357255986</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -12922,7 +12926,7 @@
       </c>
       <c r="B37" s="68">
         <f>parameters!E37</f>
-        <v>-0.18</v>
+        <v>0.88289246625534823</v>
       </c>
       <c r="C37" s="67">
         <f>parameters!G37</f>
@@ -12930,15 +12934,15 @@
       </c>
       <c r="D37" s="69">
         <f>parameters!H37</f>
-        <v>-0.18</v>
+        <v>0.88289246625534823</v>
       </c>
       <c r="E37" s="69">
         <f>parameters!I37</f>
-        <v>6.1225614830958487E-2</v>
+        <v>3.5594818478965271E-2</v>
       </c>
       <c r="F37" s="69">
         <f>parameters!J37</f>
-        <v>-0.18</v>
+        <v>0.88289246625534823</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -12948,7 +12952,7 @@
       </c>
       <c r="B38" s="68">
         <f>parameters!E38</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38" s="67">
         <f>parameters!G38</f>
@@ -12956,15 +12960,15 @@
       </c>
       <c r="D38" s="69">
         <f>parameters!H38</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" s="69">
         <f>parameters!I38</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" s="69">
         <f>parameters!J38</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -13523,14 +13527,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="193" t="s">
+      <c r="A1" s="194" t="s">
         <v>261</v>
       </c>
-      <c r="B1" s="194"/>
-      <c r="C1" s="194"/>
-      <c r="D1" s="194"/>
-      <c r="E1" s="194"/>
-      <c r="F1" s="194"/>
+      <c r="B1" s="195"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
+      <c r="E1" s="195"/>
+      <c r="F1" s="195"/>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="115"/>
@@ -16010,18 +16014,18 @@
         <v>374</v>
       </c>
       <c r="H77" s="161"/>
-      <c r="I77" s="195" t="s">
+      <c r="I77" s="196" t="s">
         <v>73</v>
       </c>
-      <c r="J77" s="195"/>
-      <c r="K77" s="195"/>
-      <c r="L77" s="195"/>
-      <c r="M77" s="195" t="s">
+      <c r="J77" s="196"/>
+      <c r="K77" s="196"/>
+      <c r="L77" s="196"/>
+      <c r="M77" s="196" t="s">
         <v>74</v>
       </c>
-      <c r="N77" s="195"/>
-      <c r="O77" s="195"/>
-      <c r="P77" s="195"/>
+      <c r="N77" s="196"/>
+      <c r="O77" s="196"/>
+      <c r="P77" s="196"/>
     </row>
     <row r="78" spans="1:17" ht="15.75">
       <c r="A78" s="175" t="s">
@@ -18141,38 +18145,38 @@
       <c r="A1" s="143"/>
       <c r="B1" s="144"/>
       <c r="C1" s="145"/>
-      <c r="D1" s="196" t="s">
+      <c r="D1" s="197" t="s">
         <v>288</v>
       </c>
-      <c r="E1" s="197"/>
-      <c r="F1" s="197"/>
-      <c r="G1" s="197"/>
-      <c r="H1" s="197"/>
-      <c r="I1" s="197"/>
-      <c r="J1" s="197"/>
-      <c r="K1" s="197"/>
-      <c r="L1" s="197"/>
-      <c r="M1" s="197"/>
-      <c r="N1" s="197"/>
-      <c r="O1" s="197"/>
-      <c r="P1" s="197"/>
-      <c r="Q1" s="198"/>
-      <c r="R1" s="199" t="s">
+      <c r="E1" s="198"/>
+      <c r="F1" s="198"/>
+      <c r="G1" s="198"/>
+      <c r="H1" s="198"/>
+      <c r="I1" s="198"/>
+      <c r="J1" s="198"/>
+      <c r="K1" s="198"/>
+      <c r="L1" s="198"/>
+      <c r="M1" s="198"/>
+      <c r="N1" s="198"/>
+      <c r="O1" s="198"/>
+      <c r="P1" s="198"/>
+      <c r="Q1" s="199"/>
+      <c r="R1" s="200" t="s">
         <v>289</v>
       </c>
-      <c r="S1" s="200"/>
-      <c r="T1" s="200"/>
-      <c r="U1" s="200"/>
-      <c r="V1" s="200"/>
-      <c r="W1" s="200"/>
-      <c r="X1" s="200"/>
-      <c r="Y1" s="200"/>
-      <c r="Z1" s="200"/>
-      <c r="AA1" s="200"/>
-      <c r="AB1" s="200"/>
-      <c r="AC1" s="200"/>
-      <c r="AD1" s="200"/>
-      <c r="AE1" s="200"/>
+      <c r="S1" s="201"/>
+      <c r="T1" s="201"/>
+      <c r="U1" s="201"/>
+      <c r="V1" s="201"/>
+      <c r="W1" s="201"/>
+      <c r="X1" s="201"/>
+      <c r="Y1" s="201"/>
+      <c r="Z1" s="201"/>
+      <c r="AA1" s="201"/>
+      <c r="AB1" s="201"/>
+      <c r="AC1" s="201"/>
+      <c r="AD1" s="201"/>
+      <c r="AE1" s="201"/>
     </row>
     <row r="2" spans="1:31">
       <c r="A2" s="147" t="s">
@@ -20110,7 +20114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{163FD219-33FE-4B73-93FF-8BB9FDED9434}">
   <dimension ref="A1:AB16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
@@ -21729,8 +21733,8 @@
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
       <c r="J1" s="8"/>
-      <c r="K1" s="201"/>
-      <c r="L1" s="194"/>
+      <c r="K1" s="202"/>
+      <c r="L1" s="195"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="7"/>
@@ -21785,21 +21789,21 @@
       <c r="A6" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="202" t="s">
+      <c r="B6" s="203" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="202"/>
-      <c r="D6" s="202"/>
-      <c r="E6" s="202"/>
-      <c r="F6" s="202"/>
+      <c r="C6" s="203"/>
+      <c r="D6" s="203"/>
+      <c r="E6" s="203"/>
+      <c r="F6" s="203"/>
       <c r="G6" s="15"/>
-      <c r="H6" s="202" t="s">
+      <c r="H6" s="203" t="s">
         <v>74</v>
       </c>
-      <c r="I6" s="202"/>
-      <c r="J6" s="202"/>
-      <c r="K6" s="202"/>
-      <c r="L6" s="202"/>
+      <c r="I6" s="203"/>
+      <c r="J6" s="203"/>
+      <c r="K6" s="203"/>
+      <c r="L6" s="203"/>
     </row>
     <row r="7" spans="1:12" ht="18.75">
       <c r="A7" s="16" t="s">
@@ -25782,13 +25786,13 @@
       </c>
       <c r="K2" s="39"/>
       <c r="L2" s="39"/>
-      <c r="N2" s="203" t="s">
+      <c r="N2" s="204" t="s">
         <v>89</v>
       </c>
-      <c r="O2" s="194"/>
-      <c r="P2" s="194"/>
-      <c r="Q2" s="194"/>
-      <c r="R2" s="194"/>
+      <c r="O2" s="195"/>
+      <c r="P2" s="195"/>
+      <c r="Q2" s="195"/>
+      <c r="R2" s="195"/>
       <c r="T2" t="s">
         <v>92</v>
       </c>

</xml_diff>